<commit_message>
Models: FormData TableRow Templates to Entity
</commit_message>
<xml_diff>
--- a/src/main/resources/templates/excel_templates/vat_new_invoice_fact.xlsx
+++ b/src/main/resources/templates/excel_templates/vat_new_invoice_fact.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\petra\IdeaProjects\Spring_Labs\automated_document_template_filling_system\src\main\resources\templates\excel_templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9542269-B9DA-4541-8414-95057F5231F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E11F356-2C67-4F78-B6B0-8CA9D4948B6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19095" windowHeight="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -337,7 +337,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -424,11 +424,109 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -445,17 +543,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -470,63 +559,64 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -556,6 +646,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -860,13 +981,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U32"/>
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="11.875" style="2" customWidth="1"/>
@@ -888,46 +1009,46 @@
     <col min="20" max="21" width="7" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O1" s="48" t="s">
+    <row r="1" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-    </row>
-    <row r="2" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O2" s="48" t="s">
+      <c r="P1" s="44"/>
+      <c r="Q1" s="44"/>
+      <c r="R1" s="44"/>
+    </row>
+    <row r="2" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="44" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-    </row>
-    <row r="3" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O3" s="48" t="s">
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+    </row>
+    <row r="3" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O3" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="P3" s="48"/>
-      <c r="Q3" s="48"/>
-      <c r="R3" s="48"/>
-    </row>
-    <row r="4" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="O4" s="48" t="s">
+      <c r="P3" s="44"/>
+      <c r="Q3" s="44"/>
+      <c r="R3" s="44"/>
+    </row>
+    <row r="4" spans="1:18" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O4" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="P4" s="48"/>
-      <c r="Q4" s="48"/>
-      <c r="R4" s="48"/>
-    </row>
-    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="44" t="s">
+      <c r="P4" s="44"/>
+      <c r="Q4" s="44"/>
+      <c r="R4" s="44"/>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
@@ -935,9 +1056,9 @@
       <c r="I7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="46"/>
-      <c r="K7" s="46"/>
-      <c r="L7" s="46"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="42"/>
       <c r="M7" s="6" t="s">
         <v>7</v>
       </c>
@@ -947,14 +1068,14 @@
       <c r="Q7" s="7"/>
       <c r="R7" s="7"/>
     </row>
-    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="44" t="s">
+    <row r="8" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
+      <c r="C8" s="40"/>
+      <c r="D8" s="40"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3" t="s">
         <v>5</v>
       </c>
@@ -962,9 +1083,9 @@
       <c r="I8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
+      <c r="J8" s="43"/>
+      <c r="K8" s="43"/>
+      <c r="L8" s="43"/>
       <c r="M8" s="6" t="s">
         <v>9</v>
       </c>
@@ -974,7 +1095,7 @@
       <c r="Q8" s="7"/>
       <c r="R8" s="7"/>
     </row>
-    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -994,21 +1115,21 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
-      <c r="J10" s="40"/>
-      <c r="K10" s="40"/>
-      <c r="L10" s="40"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+      <c r="H10" s="36"/>
+      <c r="I10" s="36"/>
+      <c r="J10" s="36"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="36"/>
       <c r="M10" s="6" t="s">
         <v>11</v>
       </c>
@@ -1018,21 +1139,21 @@
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
     </row>
-    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="40"/>
-      <c r="I11" s="40"/>
-      <c r="J11" s="40"/>
-      <c r="K11" s="40"/>
-      <c r="L11" s="40"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
       <c r="M11" s="6" t="s">
         <v>13</v>
       </c>
@@ -1042,21 +1163,21 @@
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
     </row>
-    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="41" t="s">
+    <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B12" s="41"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
-      <c r="J12" s="42"/>
-      <c r="K12" s="42"/>
-      <c r="L12" s="42"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
       <c r="M12" s="6" t="s">
         <v>15</v>
       </c>
@@ -1066,21 +1187,21 @@
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
     </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="41"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="42"/>
-      <c r="J13" s="42"/>
-      <c r="K13" s="42"/>
-      <c r="L13" s="42"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
       <c r="M13" s="6" t="s">
         <v>17</v>
       </c>
@@ -1090,21 +1211,21 @@
       <c r="Q13" s="7"/>
       <c r="R13" s="7"/>
     </row>
-    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="41" t="s">
+    <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="41"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
-      <c r="H14" s="40"/>
-      <c r="I14" s="40"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="40"/>
-      <c r="L14" s="40"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="36"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
+      <c r="J14" s="36"/>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
       <c r="M14" s="6" t="s">
         <v>19</v>
       </c>
@@ -1114,23 +1235,23 @@
       <c r="Q14" s="7"/>
       <c r="R14" s="7"/>
     </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="41" t="s">
+    <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="41"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="43"/>
-      <c r="K15" s="43"/>
-      <c r="L15" s="43"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
       <c r="M15" s="6" t="s">
         <v>22</v>
       </c>
@@ -1140,21 +1261,21 @@
       <c r="Q15" s="7"/>
       <c r="R15" s="7"/>
     </row>
-    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
-      <c r="L16" s="40"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="36"/>
+      <c r="H16" s="36"/>
+      <c r="I16" s="36"/>
+      <c r="J16" s="36"/>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
       <c r="M16" s="6" t="s">
         <v>24</v>
       </c>
@@ -1164,21 +1285,21 @@
       <c r="Q16" s="7"/>
       <c r="R16" s="7"/>
     </row>
-    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="40"/>
-      <c r="C17" s="40"/>
-      <c r="D17" s="40"/>
-      <c r="E17" s="40"/>
-      <c r="F17" s="40"/>
-      <c r="G17" s="40"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36"/>
+      <c r="E17" s="36"/>
+      <c r="F17" s="36"/>
+      <c r="G17" s="36"/>
+      <c r="H17" s="36"/>
+      <c r="I17" s="36"/>
+      <c r="J17" s="36"/>
+      <c r="K17" s="36"/>
+      <c r="L17" s="36"/>
       <c r="M17" s="6" t="s">
         <v>25</v>
       </c>
@@ -1188,21 +1309,21 @@
       <c r="Q17" s="7"/>
       <c r="R17" s="7"/>
     </row>
-    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="41"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="38"/>
+      <c r="I18" s="38"/>
+      <c r="J18" s="38"/>
+      <c r="K18" s="38"/>
+      <c r="L18" s="38"/>
       <c r="M18" s="6" t="s">
         <v>27</v>
       </c>
@@ -1212,21 +1333,21 @@
       <c r="Q18" s="7"/>
       <c r="R18" s="7"/>
     </row>
-    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="41" t="s">
+    <row r="19" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="41"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="40"/>
-      <c r="F19" s="40"/>
-      <c r="G19" s="40"/>
-      <c r="H19" s="40"/>
-      <c r="I19" s="40"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="40"/>
-      <c r="L19" s="40"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
+      <c r="H19" s="36"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="36"/>
+      <c r="K19" s="36"/>
+      <c r="L19" s="36"/>
       <c r="M19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1236,7 +1357,7 @@
       <c r="Q19" s="7"/>
       <c r="R19" s="7"/>
     </row>
-    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="7" t="s">
         <v>30</v>
@@ -1282,244 +1403,275 @@
       </c>
       <c r="R20" s="7"/>
     </row>
-    <row r="21" spans="1:19" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="33" t="s">
+    <row r="21" spans="1:19" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="B21" s="34"/>
-      <c r="C21" s="33" t="s">
+      <c r="B21" s="31"/>
+      <c r="C21" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="33" t="s">
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="G21" s="33" t="s">
+      <c r="G21" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="34"/>
-      <c r="I21" s="33" t="s">
+      <c r="H21" s="31"/>
+      <c r="I21" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="J21" s="34"/>
-      <c r="K21" s="33" t="s">
+      <c r="J21" s="31"/>
+      <c r="K21" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="33" t="s">
+      <c r="L21" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="M21" s="33" t="s">
+      <c r="M21" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="N21" s="33" t="s">
+      <c r="N21" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="O21" s="34"/>
-      <c r="P21" s="33" t="s">
+      <c r="O21" s="31"/>
+      <c r="P21" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="37" t="s">
+      <c r="Q21" s="31"/>
+      <c r="R21" s="34" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="35"/>
-      <c r="B22" s="36"/>
-      <c r="C22" s="10" t="s">
+    <row r="22" spans="1:19" s="9" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
+      <c r="C22" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D22" s="38" t="s">
+      <c r="D22" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="39"/>
-      <c r="F22" s="35"/>
-      <c r="G22" s="35"/>
-      <c r="H22" s="36"/>
-      <c r="I22" s="35"/>
-      <c r="J22" s="36"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="35"/>
-      <c r="N22" s="35"/>
-      <c r="O22" s="36"/>
-      <c r="P22" s="10" t="s">
+      <c r="E22" s="31"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="33"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="32"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="Q22" s="10" t="s">
+      <c r="Q22" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="R22" s="37"/>
-      <c r="S22" s="11" t="s">
+      <c r="R22" s="35"/>
+      <c r="S22" s="10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="31" t="s">
+    <row r="23" spans="1:19" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="32"/>
-      <c r="C23" s="12" t="s">
+      <c r="B23" s="29"/>
+      <c r="C23" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="D23" s="31" t="s">
+      <c r="D23" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="E23" s="32"/>
-      <c r="F23" s="12" t="s">
+      <c r="E23" s="29"/>
+      <c r="F23" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="29" t="s">
         <v>59</v>
       </c>
-      <c r="H23" s="32"/>
-      <c r="I23" s="31" t="s">
+      <c r="H23" s="29"/>
+      <c r="I23" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="J23" s="32"/>
-      <c r="K23" s="12" t="s">
+      <c r="J23" s="29"/>
+      <c r="K23" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="L23" s="12" t="s">
+      <c r="L23" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="M23" s="12" t="s">
+      <c r="M23" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="N23" s="31" t="s">
+      <c r="N23" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="O23" s="32"/>
-      <c r="P23" s="12" t="s">
+      <c r="O23" s="29"/>
+      <c r="P23" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="Q23" s="12" t="s">
+      <c r="Q23" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="R23" s="17" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="24" t="s">
+    <row r="24" spans="1:19" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="26"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="27"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="25"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+    </row>
+    <row r="25" spans="1:19" s="9" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B24" s="25"/>
-      <c r="C24" s="25"/>
-      <c r="D24" s="25"/>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="28" t="s">
+      <c r="B25" s="46"/>
+      <c r="C25" s="46"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="50" t="s">
         <v>69</v>
       </c>
-      <c r="L24" s="29"/>
-      <c r="M24" s="14"/>
-      <c r="N24" s="30"/>
-      <c r="O24" s="30"/>
-    </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="21" t="s">
+      <c r="L25" s="51"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="49"/>
+    </row>
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="L27" s="21" t="s">
+      <c r="B28" s="52"/>
+      <c r="L28" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="M27" s="21"/>
-      <c r="N27" s="21"/>
-    </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="21" t="s">
+      <c r="M28" s="52"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22"/>
-      <c r="J28" s="22"/>
-      <c r="L28" s="21" t="s">
+      <c r="B29" s="52"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="53"/>
+      <c r="L29" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="M28" s="21"/>
-      <c r="N28" s="21"/>
-      <c r="O28" s="15"/>
-      <c r="Q28" s="22"/>
-      <c r="R28" s="22"/>
-    </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="D29" s="19" t="s">
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="12"/>
+      <c r="Q29" s="53"/>
+      <c r="R29" s="53"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="E29" s="19"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="19" t="s">
+      <c r="E30" s="23"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="O29" s="16" t="s">
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="O30" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="P29" s="18"/>
-      <c r="Q29" s="19" t="s">
+      <c r="P30" s="15"/>
+      <c r="Q30" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="R29" s="19"/>
-    </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="21" t="s">
+      <c r="R30" s="23"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="21"/>
-      <c r="C31" s="21"/>
-      <c r="D31" s="21"/>
-      <c r="E31" s="22"/>
-      <c r="F31" s="22"/>
-      <c r="H31" s="22"/>
-      <c r="I31" s="22"/>
-      <c r="J31" s="22"/>
-      <c r="K31" s="22"/>
-      <c r="M31" s="23"/>
-      <c r="N31" s="23"/>
-      <c r="O31" s="23"/>
-      <c r="P31" s="23"/>
-      <c r="Q31" s="23"/>
-      <c r="R31" s="23"/>
-    </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="E32" s="19" t="s">
+      <c r="B32" s="55"/>
+      <c r="C32" s="55"/>
+      <c r="E32" s="53"/>
+      <c r="F32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+      <c r="M32" s="54"/>
+      <c r="N32" s="54"/>
+      <c r="O32" s="54"/>
+      <c r="P32" s="54"/>
+      <c r="Q32" s="54"/>
+      <c r="R32" s="54"/>
+    </row>
+    <row r="33" spans="5:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="F32" s="19"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="19" t="s">
+      <c r="F33" s="23"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="M32" s="20" t="s">
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="M33" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="N32" s="20"/>
-      <c r="O32" s="20"/>
-      <c r="P32" s="20"/>
-      <c r="Q32" s="20"/>
-      <c r="R32" s="20"/>
+      <c r="N33" s="24"/>
+      <c r="O33" s="24"/>
+      <c r="P33" s="24"/>
+      <c r="Q33" s="24"/>
+      <c r="R33" s="24"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <mergeCells count="65">
+  <mergeCells count="63">
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="M32:R32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="H32:K32"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="G29:J29"/>
+    <mergeCell ref="L28:M28"/>
+    <mergeCell ref="L29:N29"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="K25:L25"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="A28:B28"/>
     <mergeCell ref="O1:R1"/>
     <mergeCell ref="O2:R2"/>
     <mergeCell ref="O3:R3"/>
@@ -1564,27 +1716,11 @@
     <mergeCell ref="D23:E23"/>
     <mergeCell ref="G23:H23"/>
     <mergeCell ref="I23:J23"/>
-    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="G24:H24"/>
     <mergeCell ref="I24:J24"/>
-    <mergeCell ref="K24:L24"/>
     <mergeCell ref="N24:O24"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="G29:J29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="L27:N27"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="G28:J28"/>
-    <mergeCell ref="L28:N28"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="H32:K32"/>
-    <mergeCell ref="M32:R32"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="H31:K31"/>
-    <mergeCell ref="M31:R31"/>
   </mergeCells>
   <pageMargins left="0.59055118110236005" right="0.59055118110236005" top="0.59055118110236005" bottom="0.59055118110236005" header="0.51181102362205" footer="0.51181102362205"/>
   <pageSetup paperSize="9" scale="93" orientation="landscape"/>

</xml_diff>